<commit_message>
ISD lab 2b fix
</commit_message>
<xml_diff>
--- a/labs.xlsx
+++ b/labs.xlsx
@@ -20,27 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">ИБ</t>
   </si>
   <si>
+    <t xml:space="preserve">Задачи на листе взять</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ММО</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПИСдец</t>
+  </si>
+  <si>
     <t xml:space="preserve">теория</t>
   </si>
   <si>
-    <t xml:space="preserve">ММО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ПИСдец</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default, constraint, pattern переписать 2а</t>
-  </si>
-  <si>
     <t xml:space="preserve">ПиРБДИП</t>
-  </si>
-  <si>
-    <t xml:space="preserve">отчёты</t>
   </si>
   <si>
     <t xml:space="preserve">На вопросы надо будет овтетить</t>
@@ -92,7 +89,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,14 +110,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -164,7 +167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,6 +193,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,8 +455,8 @@
   </sheetPr>
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -535,21 +542,21 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
@@ -559,8 +566,8 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -583,15 +590,13 @@
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="1"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -608,12 +613,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -632,7 +635,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -655,44 +658,44 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>

</xml_diff>